<commit_message>
Add linear fit of Gain vs Channel with error bars
</commit_message>
<xml_diff>
--- a/Data/dataset2/SiMP student data2_second trial.xlsx
+++ b/Data/dataset2/SiMP student data2_second trial.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="18820" windowHeight="8090"/>
+    <workbookView activeTab="4" windowWidth="18820" windowHeight="8090"/>
   </bookViews>
   <sheets>
     <sheet name="New-histogram (2)" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,7 @@
     <sheet name="I_V_curve" sheetId="3" r:id="rId3"/>
     <sheet name="I-V_curve_old" sheetId="4" r:id="rId4"/>
     <sheet name="100att_gain38" sheetId="5" r:id="rId5"/>
-    <sheet name="loggerpro_fit" sheetId="6" r:id="rId6"/>
-    <sheet name="newI-V_Keithley" sheetId="7" r:id="rId7"/>
+    <sheet name="newI-V_Keithley" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="solver_mrt" localSheetId="0">0.074999999999999997</definedName>
@@ -80,10 +79,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="4">"100att_gain38"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'100att_gain38'!$A$1:$R$32</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="5">"loggerpro_fit"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="5">"newI-V_Keithley"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="6">"newI-V_Keithley"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">#REF!</definedName>
   </definedNames>
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" codePage="1252"/>
@@ -2255,40 +2252,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>460815</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>238123</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -2357,8 +2320,8 @@
   </sheetPr>
   <dimension ref="A1:J4096"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="60" tabSelected="1">
-      <selection activeCell="P54" sqref="P54"/>
+    <sheetView workbookViewId="0" zoomScale="60">
+      <selection activeCell="A1" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -53579,8 +53542,8 @@
   </sheetPr>
   <dimension ref="A1:U2404"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="80">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0" zoomScale="80" tabSelected="1">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -73135,35 +73098,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:V39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" style="1" width="9.142307692307693"/>
-    <col min="2" max="16384" style="1" width="9.142307692307693"/>
-  </cols>
-  <sheetData/>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
-  <headerFooter>
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>

</xml_diff>